<commit_message>
changed the sample excel files
</commit_message>
<xml_diff>
--- a/public/Sample_Company_Masters.xlsx
+++ b/public/Sample_Company_Masters.xlsx
@@ -19,25 +19,25 @@
     <t>BSE</t>
   </si>
   <si>
-    <t>Name of the Company(as per certificate)</t>
-  </si>
-  <si>
-    <t>Current Name of the Company</t>
-  </si>
-  <si>
-    <t>ISIN</t>
+    <t>Name of the Company(as per certificate)*</t>
+  </si>
+  <si>
+    <t>Current Name of the Company*</t>
+  </si>
+  <si>
+    <t>ISIN*</t>
   </si>
   <si>
     <t>CIN</t>
   </si>
   <si>
-    <t>Face Value</t>
-  </si>
-  <si>
-    <t>Closing Price in NSE</t>
-  </si>
-  <si>
-    <t>Closing Price in BSE</t>
+    <t>Face Value*</t>
+  </si>
+  <si>
+    <t>Closing Price in NSE*</t>
+  </si>
+  <si>
+    <t>Closing Price in BSE*</t>
   </si>
   <si>
     <t>Registered Office</t>
@@ -119,27 +119,27 @@
     <border/>
     <border>
       <left style="thin">
-        <color rgb="FF888888"/>
+        <color rgb="FF757575"/>
       </left>
       <right style="thin">
-        <color rgb="FF888888"/>
+        <color rgb="FF757575"/>
       </right>
       <top style="thin">
-        <color rgb="FF888888"/>
+        <color rgb="FF757575"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF888888"/>
+        <color rgb="FF757575"/>
       </bottom>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF888888"/>
+        <color rgb="FF757575"/>
       </left>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color rgb="FF888888"/>
+        <color rgb="FF757575"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
@@ -153,7 +153,7 @@
         <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color rgb="FF888888"/>
+        <color rgb="FF757575"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
@@ -164,10 +164,10 @@
         <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color rgb="FF888888"/>
+        <color rgb="FF757575"/>
       </right>
       <top style="thin">
-        <color rgb="FF888888"/>
+        <color rgb="FF757575"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
@@ -177,7 +177,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -192,6 +192,9 @@
     </xf>
     <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
@@ -506,13 +509,13 @@
         <v>3990.0</v>
       </c>
       <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
       <c r="M2" s="5"/>
       <c r="N2" s="5"/>
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
+      <c r="Q2" s="6"/>
       <c r="R2" s="5"/>
       <c r="S2" s="5"/>
       <c r="T2" s="5"/>

</xml_diff>